<commit_message>
Item Data Load Test & Item XML 작성
</commit_message>
<xml_diff>
--- a/ZombieProject/Assets/Project/Resources/Data/Item/XLSX/ItemData.xlsx
+++ b/ZombieProject/Assets/Project/Resources/Data/Item/XLSX/ItemData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProject\FinalZombieProject\ZombieProject\Assets\Project\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProject\FinalZombieProject\ZombieProject\Assets\Project\Resources\Data\Item\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A4BEEE-22F4-4ED9-94E4-D302C8830DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70406361-1EDF-46B3-9E42-00F92B0014A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{B0978E18-6600-4397-BD5C-3FB47AEF09D0}"/>
   </bookViews>
@@ -35,20 +35,23 @@
   <connection id="1" xr16:uid="{F900ABFD-A840-4016-9974-55B10366896A}" name="itemData" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\UnityProject\FinalZombieProject\ZombieProject\Assets\Project\Resources\Data\itemData.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" xr16:uid="{1CEB10B8-F995-4084-835F-385DF1662B82}" name="itemData1" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{D80641EF-6D05-4ED1-A119-D7013D001FBC}" name="itemData_Schema" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\UnityProject\FinalZombieProject\ZombieProject\Assets\Project\Resources\Data\Item\Schema\itemData_Schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="3" xr16:uid="{1CEB10B8-F995-4084-835F-385DF1662B82}" name="itemData1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\UnityProject\FinalZombieProject\ZombieProject\Assets\Project\Resources\Data\itemData.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" xr16:uid="{79646CCE-EDA5-4F13-A3BB-0384E3C6C7CC}" name="itemData2" type="4" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{79646CCE-EDA5-4F13-A3BB-0384E3C6C7CC}" name="itemData2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\UnityProject\FinalZombieProject\ZombieProject\Assets\Project\Resources\Data\itemData.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="4" xr16:uid="{D03A2632-3C91-4E02-AD24-ECD008D647CF}" name="itemData3" type="4" refreshedVersion="0" background="1">
+  <connection id="5" xr16:uid="{D03A2632-3C91-4E02-AD24-ECD008D647CF}" name="itemData3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\UnityProject\FinalZombieProject\ZombieProject\Assets\Project\Resources\Data\itemData.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>ItemID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +118,18 @@
   </si>
   <si>
     <t>MELEE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FALSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Armor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -167,14 +182,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -187,7 +199,10 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -245,7 +260,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema2">
+  <Schema ID="Schema3">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Root">
         <xsd:complexType>
@@ -274,82 +289,54 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema5">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="root">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Item" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="ItemID" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ItemName" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="IconName" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ModelName" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ItemSort" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="HP" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Attack" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="MovePoint" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="HPRegenerate" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Range" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="isAccumulate" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="AttackSpeed" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Map ID="5" Name="root_맵" RootElement="root" SchemaID="Schema5" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
-  </Map>
-  <Map ID="2" Name="Root_맵" RootElement="Root" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+  <Map ID="7" Name="Root_맵" RootElement="Root" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FF4CB01-9852-4F47-B179-3FCC4383DB1F}" name="표1" displayName="표1" ref="A1:L4" tableType="xml" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" connectionId="4">
-  <autoFilter ref="A1:L4" xr:uid="{E08CC164-3B86-4B67-B78D-AA82DD77E89B}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A1A6487F-6539-41FE-B783-1612934EEAE2}" uniqueName="ItemID" name="ItemID" dataDxfId="11">
-      <xmlColumnPr mapId="5" xpath="/root/Item/ItemID" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{75ADB0AE-67A7-4A6B-A46C-4543A386AAC7}" uniqueName="ItemName" name="ItemName" dataDxfId="10">
-      <xmlColumnPr mapId="5" xpath="/root/Item/ItemName" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{1C9BEB4B-06E1-4117-9548-98DEF7E14AA4}" uniqueName="IconName" name="IconName" dataDxfId="9">
-      <xmlColumnPr mapId="5" xpath="/root/Item/IconName" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{D46C489D-D7D1-4178-A0CF-55DE5E4CBE19}" uniqueName="ModelName" name="ModelName" dataDxfId="8">
-      <xmlColumnPr mapId="5" xpath="/root/Item/ModelName" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{7C8EF2FD-5A01-4867-A9D7-04A7FD349504}" uniqueName="ItemSort" name="ItemSort" dataDxfId="7">
-      <xmlColumnPr mapId="5" xpath="/root/Item/ItemSort" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{03E4D02F-3F9F-42AB-B47A-BC7819427D4E}" uniqueName="HP" name="HP" dataDxfId="6">
-      <xmlColumnPr mapId="5" xpath="/root/Item/HP" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{20F3625B-54EE-4954-B717-BC1AFD106BB1}" uniqueName="Attack" name="Attack" dataDxfId="5">
-      <xmlColumnPr mapId="5" xpath="/root/Item/Attack" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{7EA77745-B4B2-4E40-9053-5428DC18074E}" uniqueName="MovePoint" name="MovePoint" dataDxfId="4">
-      <xmlColumnPr mapId="5" xpath="/root/Item/MovePoint" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{29552D49-C9E4-468E-A2F7-A2BACCB3D3AB}" uniqueName="HPRegenerate" name="HPRegenerate" dataDxfId="3">
-      <xmlColumnPr mapId="5" xpath="/root/Item/HPRegenerate" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{1B1605FA-A793-4DAF-9B30-3D7E3EF725F8}" uniqueName="Range" name="Range" dataDxfId="2">
-      <xmlColumnPr mapId="5" xpath="/root/Item/Range" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="11" xr3:uid="{2FD5848E-748A-4FB7-9189-06BCF73D76B8}" uniqueName="isAccumulate" name="isAccumulate" dataDxfId="1">
-      <xmlColumnPr mapId="5" xpath="/root/Item/isAccumulate" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{1ABD43A8-9DAF-4C4F-B960-A8A66318512F}" uniqueName="AttackSpeed" name="AttackSpeed" dataDxfId="0">
-      <xmlColumnPr mapId="5" xpath="/root/Item/AttackSpeed" xmlDataType="integer"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FF4CB01-9852-4F47-B179-3FCC4383DB1F}" name="표1" displayName="표1" ref="A1:M4" tableType="xml" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" connectionId="2">
+  <autoFilter ref="A1:M4" xr:uid="{E08CC164-3B86-4B67-B78D-AA82DD77E89B}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{A1A6487F-6539-41FE-B783-1612934EEAE2}" uniqueName="ItemID" name="ItemID" dataDxfId="12">
+      <xmlColumnPr mapId="7" xpath="/Root/text/ItemID" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{75ADB0AE-67A7-4A6B-A46C-4543A386AAC7}" uniqueName="ItemName" name="ItemName" dataDxfId="11">
+      <xmlColumnPr mapId="7" xpath="/Root/text/ItemName" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{1C9BEB4B-06E1-4117-9548-98DEF7E14AA4}" uniqueName="IconName" name="IconName" dataDxfId="10">
+      <xmlColumnPr mapId="7" xpath="/Root/text/IconName" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{D46C489D-D7D1-4178-A0CF-55DE5E4CBE19}" uniqueName="ModelName" name="ModelName" dataDxfId="9">
+      <xmlColumnPr mapId="7" xpath="/Root/text/ModelName" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{7C8EF2FD-5A01-4867-A9D7-04A7FD349504}" uniqueName="ItemSort" name="ItemSort" dataDxfId="8">
+      <xmlColumnPr mapId="7" xpath="/Root/text/ItemSort" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{03E4D02F-3F9F-42AB-B47A-BC7819427D4E}" uniqueName="HP" name="HP" dataDxfId="7">
+      <xmlColumnPr mapId="7" xpath="/Root/text/HP" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{20F3625B-54EE-4954-B717-BC1AFD106BB1}" uniqueName="Attack" name="Attack" dataDxfId="6">
+      <xmlColumnPr mapId="7" xpath="/Root/text/Attack" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7EA77745-B4B2-4E40-9053-5428DC18074E}" uniqueName="MovePoint" name="MovePoint" dataDxfId="5">
+      <xmlColumnPr mapId="7" xpath="/Root/text/MovePoint" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{29552D49-C9E4-468E-A2F7-A2BACCB3D3AB}" uniqueName="HPRegenerate" name="HPRegenerate" dataDxfId="4">
+      <xmlColumnPr mapId="7" xpath="/Root/text/HPRegenerate" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{1B1605FA-A793-4DAF-9B30-3D7E3EF725F8}" uniqueName="Range" name="Range" dataDxfId="3">
+      <xmlColumnPr mapId="7" xpath="/Root/text/Range" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{2FD5848E-748A-4FB7-9189-06BCF73D76B8}" uniqueName="isAccumulate" name="isAccumulate" dataDxfId="2">
+      <xmlColumnPr mapId="7" xpath="/Root/text/isAccumulate" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{1ABD43A8-9DAF-4C4F-B960-A8A66318512F}" uniqueName="AttackSpeed" name="AttackSpeed" dataDxfId="1">
+      <xmlColumnPr mapId="7" xpath="/Root/text/AttackSpeed" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{9E9C2C4F-0384-48D0-8406-E4C4969CBB1D}" uniqueName="Armor" name="Armor" dataDxfId="0">
+      <xmlColumnPr mapId="7" xpath="/Root/text/Armor" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -655,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE82CDF-E403-47D3-95A5-30B9A0F7BF8C}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -667,12 +654,13 @@
     <col min="4" max="4" width="16.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
@@ -712,85 +700,91 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="K2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
         <v>5</v>
       </c>
-      <c r="M2" s="3"/>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
         <v>1</v>
       </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2">
         <v>10</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
@@ -823,13 +817,15 @@
       <c r="J4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L4" s="2">
         <v>12</v>
       </c>
-      <c r="M4" s="2"/>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>